<commit_message>
tax analysis (fig 1) + kegg analysis (fig 2)
</commit_message>
<xml_diff>
--- a/04_immune_genes/KEGG 5-1 immune system.xlsx
+++ b/04_immune_genes/KEGG 5-1 immune system.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="ton"/>
+  <fileSharing readOnlyRecommended="0" userName="drozdovapb"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="11180" windowHeight="11023" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="11174" windowHeight="11016" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId4"/>
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1743341337" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1743341337" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1743341337" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1743341337"/>
+      <pm:revision xmlns:pm="smNativeData" day="1743493018" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1743493018" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1743493018" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1743493018"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -37,10 +37,16 @@
     <t>Not in Amparyup 2020</t>
   </si>
   <si>
+    <t>Date added in KEGG</t>
+  </si>
+  <si>
     <t>map04640</t>
   </si>
   <si>
     <t>Hematopoietic cell lineage</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>map04610</t>
@@ -179,15 +185,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;₽&quot;;\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₽&quot;;[Red]\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₽&quot;;\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+  <numFmts count="9">
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -197,7 +204,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1743341337" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1743493018" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -212,7 +219,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1743341337" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1743493018" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -227,7 +234,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1743341337" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1743493018" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="240" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -243,7 +250,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1743341337" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1743493018" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -252,7 +259,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,13 +272,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1743341337" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1743493018" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF9E"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1743493018" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -287,7 +305,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1743341337"/>
+          <pm:border xmlns:pm="smNativeData" id="1743493018"/>
         </ext>
       </extLst>
     </border>
@@ -306,7 +324,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1743341337"/>
+          <pm:border xmlns:pm="smNativeData" id="1743493018"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1743493018"/>
         </ext>
       </extLst>
     </border>
@@ -314,12 +351,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -327,8 +378,8 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1743341337" count="1">
-        <pm:charStyle name="Обычный" fontId="0" Id="1"/>
+      <pm:charStyles xmlns:pm="smNativeData" id="1743493018" count="1">
+        <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
   </extLst>
@@ -591,19 +642,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="10.901786" customWidth="1"/>
     <col min="3" max="3" width="37.526786" customWidth="1"/>
+    <col min="5" max="5" width="10.000000" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,249 +668,317 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E4" s="3" t="n">
+        <v>41757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="12" t="n">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>42613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>40113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>40072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E10" s="5" t="n">
+        <v>40146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>38756</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>42688</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>42718</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>42746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>38775</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>45</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>38953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>40172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>38885</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1743341337" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1743493018" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -867,14 +987,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1743341337" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1743341337" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1743493018" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1743493018" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1743341337" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1743493018" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>